<commit_message>
add cache miss and CPI
</commit_message>
<xml_diff>
--- a/excel.xlsx
+++ b/excel.xlsx
@@ -8,15 +8,46 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Phol\Desktop\github\Parallel_shell_sort_comarch_assignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7115CD86-D718-4987-955B-657C5669E018}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{864F6870-754E-40A7-A7C1-B8B3518B77B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{4A95CAEF-9012-45F3-BF0F-ABD0891E4093}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">(Sheet1!$C$27,Sheet1!$E$27,Sheet1!$G$27,Sheet1!$I$27)</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">(Sheet1!$C$29,Sheet1!$E$29,Sheet1!$G$29,Sheet1!$I$29)</definedName>
+    <definedName name="_xlchart.v1.10" hidden="1">Sheet1!$C$24</definedName>
+    <definedName name="_xlchart.v1.11" hidden="1">Sheet1!$D$24</definedName>
+    <definedName name="_xlchart.v1.12" hidden="1">(Sheet1!$C$27,Sheet1!$E$27,Sheet1!$G$27,Sheet1!$I$27)</definedName>
+    <definedName name="_xlchart.v1.13" hidden="1">(Sheet1!$C$29,Sheet1!$E$29,Sheet1!$G$29,Sheet1!$I$29)</definedName>
+    <definedName name="_xlchart.v1.14" hidden="1">(Sheet1!$D$27,Sheet1!$F$27,Sheet1!$H$27,Sheet1!$J$27)</definedName>
+    <definedName name="_xlchart.v1.15" hidden="1">(Sheet1!$D$29,Sheet1!$F$29,Sheet1!$H$29,Sheet1!$J$29)</definedName>
+    <definedName name="_xlchart.v1.16" hidden="1">Sheet1!$C$24</definedName>
+    <definedName name="_xlchart.v1.17" hidden="1">Sheet1!$D$24</definedName>
+    <definedName name="_xlchart.v1.18" hidden="1">(Sheet1!$C$27,Sheet1!$E$27,Sheet1!$G$27,Sheet1!$I$27)</definedName>
+    <definedName name="_xlchart.v1.19" hidden="1">(Sheet1!$C$29,Sheet1!$E$29,Sheet1!$G$29,Sheet1!$I$29)</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">(Sheet1!$D$27,Sheet1!$F$27,Sheet1!$H$27,Sheet1!$J$27)</definedName>
+    <definedName name="_xlchart.v1.20" hidden="1">(Sheet1!$D$27,Sheet1!$F$27,Sheet1!$H$27,Sheet1!$J$27)</definedName>
+    <definedName name="_xlchart.v1.21" hidden="1">(Sheet1!$D$29,Sheet1!$F$29,Sheet1!$H$29,Sheet1!$J$29)</definedName>
+    <definedName name="_xlchart.v1.22" hidden="1">Sheet1!$C$24</definedName>
+    <definedName name="_xlchart.v1.23" hidden="1">Sheet1!$D$24</definedName>
+    <definedName name="_xlchart.v1.24" hidden="1">(Sheet1!$C$27,Sheet1!$E$27,Sheet1!$G$27,Sheet1!$I$27)</definedName>
+    <definedName name="_xlchart.v1.25" hidden="1">(Sheet1!$C$29,Sheet1!$E$29,Sheet1!$G$29,Sheet1!$I$29)</definedName>
+    <definedName name="_xlchart.v1.26" hidden="1">(Sheet1!$D$27,Sheet1!$F$27,Sheet1!$H$27,Sheet1!$J$27)</definedName>
+    <definedName name="_xlchart.v1.27" hidden="1">(Sheet1!$D$29,Sheet1!$F$29,Sheet1!$H$29,Sheet1!$J$29)</definedName>
+    <definedName name="_xlchart.v1.28" hidden="1">Sheet1!$C$24</definedName>
+    <definedName name="_xlchart.v1.29" hidden="1">Sheet1!$D$24</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">(Sheet1!$D$29,Sheet1!$F$29,Sheet1!$H$29,Sheet1!$J$29)</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">Sheet1!$C$24</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">Sheet1!$D$24</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">(Sheet1!$C$27,Sheet1!$E$27,Sheet1!$G$27,Sheet1!$I$27)</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">(Sheet1!$C$29,Sheet1!$E$29,Sheet1!$G$29,Sheet1!$I$29)</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">(Sheet1!$D$27,Sheet1!$F$27,Sheet1!$H$27,Sheet1!$J$27)</definedName>
+    <definedName name="_xlchart.v1.9" hidden="1">(Sheet1!$D$29,Sheet1!$F$29,Sheet1!$H$29,Sheet1!$J$29)</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="38">
   <si>
     <t>cpu-cycles</t>
   </si>
@@ -145,7 +176,10 @@
     <t>Branch-Load-Misses</t>
   </si>
   <si>
-    <t>Time</t>
+    <t>Time (s)</t>
+  </si>
+  <si>
+    <t>CPI</t>
   </si>
 </sst>
 </file>
@@ -312,7 +346,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>CPU-Cycles</a:t>
+              <a:t>CPI</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -465,21 +499,21 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>(Sheet1!$C$25,Sheet1!$E$25,Sheet1!$G$25,Sheet1!$I$25)</c:f>
+              <c:f>(Sheet1!$C$27,Sheet1!$E$27,Sheet1!$G$27,Sheet1!$I$27)</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>59.391411425999998</c:v>
+                  <c:v>0.57296623222631882</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>64.357536593000006</c:v>
+                  <c:v>0.60779002570999463</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>78.371448963999995</c:v>
+                  <c:v>0.71994948656167612</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>114.663656015</c:v>
+                  <c:v>1.0189850145660018</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -556,7 +590,7 @@
                 <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
-            <c:dLblPos val="t"/>
+            <c:dLblPos val="b"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
             <c:showCatName val="0"/>
@@ -607,21 +641,21 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>(Sheet1!$D$25,Sheet1!$F$25,Sheet1!$H$25,Sheet1!$J$25)</c:f>
+              <c:f>(Sheet1!$D$27,Sheet1!$F$27,Sheet1!$H$27,Sheet1!$J$27)</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>135.23394950599999</c:v>
+                  <c:v>0.55703197754460287</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>142.864446673</c:v>
+                  <c:v>0.58404278261349118</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>159.75272822400001</c:v>
+                  <c:v>0.64402153921393268</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>243.81461345100001</c:v>
+                  <c:v>0.95190701791986332</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -634,7 +668,7 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="t"/>
+          <c:dLblPos val="r"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="1"/>
           <c:showCatName val="0"/>
@@ -783,7 +817,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>CPU-Cycles (x10^9)  </a:t>
+                  <a:t>CPI)  </a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -792,8 +826,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="2.3205685230244737E-2"/>
-              <c:y val="0.33952103814087042"/>
+              <c:x val="1.8854792982177262E-2"/>
+              <c:y val="0.42185853237713283"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -939,7 +973,940 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1680" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="bg1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>CPI and Cache-Misses</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1680" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$24</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>x</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="00B0F0"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="00B0F0"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:srgbClr val="00B0F0"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t>1 thread</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="b"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000008-A791-459F-8658-788148D369EE}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t>2 threads</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="b"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000009-A791-459F-8658-788148D369EE}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t>4 threads</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="b"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000A-A791-459F-8658-788148D369EE}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t>8 threads</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="b"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000B-A791-459F-8658-788148D369EE}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="bg1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="b"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>(Sheet1!$C$29,Sheet1!$E$29,Sheet1!$G$29,Sheet1!$I$29)</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>14.34595</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.7598099999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.9551500000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.0392900000000003</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>(Sheet1!$C$27,Sheet1!$E$27,Sheet1!$G$27,Sheet1!$I$27)</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.57296623222631882</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.60779002570999463</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.71994948656167612</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.0189850145660018</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-A791-459F-8658-788148D369EE}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$24</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>2x</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:t>1 thread</a:t>
+                    </a:r>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="t"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000004-A791-459F-8658-788148D369EE}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:t>2 threads</a:t>
+                    </a:r>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="t"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000005-A791-459F-8658-788148D369EE}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:t>4 threads</a:t>
+                    </a:r>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="t"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000006-A791-459F-8658-788148D369EE}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:t>8 threads</a:t>
+                    </a:r>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="t"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000007-A791-459F-8658-788148D369EE}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="bg1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>(Sheet1!$D$29,Sheet1!$F$29,Sheet1!$H$29,Sheet1!$J$29)</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>18.0578</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>29.023669999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10.9635</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>22.683689999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>(Sheet1!$D$27,Sheet1!$F$27,Sheet1!$H$27,Sheet1!$J$27)</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.55703197754460287</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.58404278261349118</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.64402153921393268</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.95190701791986332</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-A791-459F-8658-788148D369EE}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="t"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1923717359"/>
+        <c:axId val="1923716527"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1923717359"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="bg1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Cache-Misses (x10^5)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="bg1"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="bg1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1923716527"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1923716527"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="bg1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>CPI</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="bg1"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="bg1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1923717359"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="accent6">
+        <a:lumMod val="50000"/>
+      </a:schemeClr>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1400">
+          <a:solidFill>
+            <a:schemeClr val="bg1"/>
+          </a:solidFill>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1482,6 +2449,522 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
@@ -1886,12 +3369,12 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>1330187</xdr:colOff>
-      <xdr:row>26</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>35615</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="502702" cy="175369"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-      <mc:Choice Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="4" name="TextBox 3">
@@ -1905,7 +3388,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="2949437" y="4550465"/>
+              <a:off x="2955040" y="4663644"/>
               <a:ext cx="502702" cy="175369"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -2005,7 +3488,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback xmlns="">
+      <mc:Fallback>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="4" name="TextBox 3">
@@ -2019,7 +3502,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="2949437" y="4550465"/>
+              <a:off x="2955040" y="4663644"/>
               <a:ext cx="502702" cy="175369"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -2047,13 +3530,14 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a:r>
                 <a:rPr lang="en-US" sz="1100" i="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1"/>
                   </a:solidFill>
                   <a:effectLst/>
-                  <a:latin typeface="+mn-lt"/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                   <a:ea typeface="+mn-ea"/>
                   <a:cs typeface="+mn-cs"/>
                 </a:rPr>
@@ -2065,35 +3549,11 @@
                     <a:schemeClr val="tx1"/>
                   </a:solidFill>
                   <a:effectLst/>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:rPr>
-                <a:t>(×10〗^</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="en-US" sz="1100" b="0" i="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1"/>
-                  </a:solidFill>
-                  <a:effectLst/>
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                   <a:ea typeface="+mn-ea"/>
                   <a:cs typeface="+mn-cs"/>
                 </a:rPr>
-                <a:t>6</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="en-US" sz="1100" b="0" i="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1"/>
-                  </a:solidFill>
-                  <a:effectLst/>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:rPr>
-                <a:t>)</a:t>
+                <a:t>(×10〗^6)</a:t>
               </a:r>
               <a:endParaRPr lang="en-US">
                 <a:effectLst/>
@@ -2109,7 +3569,7 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>1025801</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:row>28</xdr:row>
       <xdr:rowOff>44726</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="502702" cy="177741"/>
@@ -2332,7 +3792,7 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>890794</xdr:colOff>
-      <xdr:row>28</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>40998</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="499880" cy="175369"/>
@@ -2531,7 +3991,7 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>1361660</xdr:colOff>
-      <xdr:row>29</xdr:row>
+      <xdr:row>30</xdr:row>
       <xdr:rowOff>34787</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="502702" cy="177741"/>
@@ -2754,7 +4214,7 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>904460</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="499880" cy="175369"/>
@@ -2953,7 +4413,7 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>1383609</xdr:colOff>
-      <xdr:row>31</xdr:row>
+      <xdr:row>32</xdr:row>
       <xdr:rowOff>49695</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="502702" cy="174663"/>
@@ -3176,7 +4636,7 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>828260</xdr:colOff>
-      <xdr:row>32</xdr:row>
+      <xdr:row>33</xdr:row>
       <xdr:rowOff>44726</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="502702" cy="175369"/>
@@ -3399,7 +4859,7 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>1297884</xdr:colOff>
-      <xdr:row>33</xdr:row>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>40998</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="502702" cy="174663"/>
@@ -3622,7 +5082,7 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>1045679</xdr:colOff>
-      <xdr:row>34</xdr:row>
+      <xdr:row>35</xdr:row>
       <xdr:rowOff>43068</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="502702" cy="175369"/>
@@ -3845,7 +5305,7 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>1504536</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>48866</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="502702" cy="174407"/>
@@ -4067,15 +5527,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>1034822</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>233361</xdr:rowOff>
+      <xdr:colOff>1116065</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>61911</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>989613</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>28709</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4095,6 +5555,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>50426</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>62752</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>184336</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>70037</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="16" name="Chart 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A07B92C0-E0B0-4920-9A2E-ACE1371FE3B1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -4400,10 +5896,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07BC9815-2855-4CB4-8B00-AD41286DC877}">
-  <dimension ref="A1:AF37"/>
+  <dimension ref="A1:AF38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R35" sqref="R35"/>
+    <sheetView tabSelected="1" topLeftCell="K40" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B58" sqref="B58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5467,408 +6963,445 @@
     </row>
     <row r="27" spans="2:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B27" s="8" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="C27" s="9">
-        <f>C6/A6</f>
-        <v>88.947239999999994</v>
+        <f>C4/C5</f>
+        <v>0.57296623222631882</v>
       </c>
       <c r="D27" s="9">
-        <f>D6/A6</f>
-        <v>279.67957899999999</v>
+        <f t="shared" ref="D27:J27" si="0">D4/D5</f>
+        <v>0.55703197754460287</v>
       </c>
       <c r="E27" s="9">
-        <f>E6/A6</f>
-        <v>126.56222099999999</v>
+        <f t="shared" si="0"/>
+        <v>0.60779002570999463</v>
       </c>
       <c r="F27" s="9">
-        <f>F6/A6</f>
-        <v>339.22745500000002</v>
+        <f t="shared" si="0"/>
+        <v>0.58404278261349118</v>
       </c>
       <c r="G27" s="9">
-        <f>G6/A6</f>
-        <v>209.25166400000001</v>
+        <f t="shared" si="0"/>
+        <v>0.71994948656167612</v>
       </c>
       <c r="H27" s="9">
-        <f>H6/A6</f>
-        <v>465.63318900000002</v>
+        <f t="shared" si="0"/>
+        <v>0.64402153921393268</v>
       </c>
       <c r="I27" s="9">
-        <f>I6/A6</f>
-        <v>219.563357</v>
+        <f t="shared" si="0"/>
+        <v>1.0189850145660018</v>
       </c>
       <c r="J27" s="9">
-        <f>J6/A6</f>
-        <v>506.13474400000001</v>
+        <f t="shared" si="0"/>
+        <v>0.95190701791986332</v>
       </c>
     </row>
     <row r="28" spans="2:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B28" s="10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C28" s="12">
-        <f>C7/A7</f>
-        <v>14.34595</v>
+        <f>C6/A6</f>
+        <v>88.947239999999994</v>
       </c>
       <c r="D28" s="12">
-        <f t="shared" ref="D28:D37" si="0">D7/A7</f>
-        <v>18.0578</v>
+        <f>D6/A6</f>
+        <v>279.67957899999999</v>
       </c>
       <c r="E28" s="12">
-        <f t="shared" ref="E28:E37" si="1">E7/A7</f>
-        <v>6.7598099999999999</v>
+        <f>E6/A6</f>
+        <v>126.56222099999999</v>
       </c>
       <c r="F28" s="12">
-        <f t="shared" ref="F28:F37" si="2">F7/A7</f>
-        <v>29.023669999999999</v>
+        <f>F6/A6</f>
+        <v>339.22745500000002</v>
       </c>
       <c r="G28" s="12">
-        <f t="shared" ref="G28:G37" si="3">G7/A7</f>
-        <v>3.9551500000000002</v>
+        <f>G6/A6</f>
+        <v>209.25166400000001</v>
       </c>
       <c r="H28" s="12">
-        <f t="shared" ref="H28:H37" si="4">H7/A7</f>
-        <v>10.9635</v>
+        <f>H6/A6</f>
+        <v>465.63318900000002</v>
       </c>
       <c r="I28" s="12">
-        <f t="shared" ref="I28:I37" si="5">I7/A7</f>
-        <v>5.0392900000000003</v>
+        <f>I6/A6</f>
+        <v>219.563357</v>
       </c>
       <c r="J28" s="12">
-        <f t="shared" ref="J28:J37" si="6">J7/A7</f>
-        <v>22.683689999999999</v>
+        <f>J6/A6</f>
+        <v>506.13474400000001</v>
       </c>
     </row>
     <row r="29" spans="2:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B29" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C29" s="9">
-        <f>C8/A8</f>
-        <v>51.102978159999999</v>
+        <f>C7/A7</f>
+        <v>14.34595</v>
       </c>
       <c r="D29" s="9">
-        <f t="shared" si="0"/>
-        <v>120.145670401</v>
+        <f t="shared" ref="D29:D38" si="1">D7/A7</f>
+        <v>18.0578</v>
       </c>
       <c r="E29" s="9">
-        <f t="shared" si="1"/>
-        <v>51.644393409000003</v>
+        <f t="shared" ref="E29:E38" si="2">E7/A7</f>
+        <v>6.7598099999999999</v>
       </c>
       <c r="F29" s="9">
-        <f t="shared" si="2"/>
-        <v>119.56081147800001</v>
+        <f t="shared" ref="F29:F38" si="3">F7/A7</f>
+        <v>29.023669999999999</v>
       </c>
       <c r="G29" s="9">
-        <f t="shared" si="3"/>
-        <v>51.655900987999999</v>
+        <f t="shared" ref="G29:G38" si="4">G7/A7</f>
+        <v>3.9551500000000002</v>
       </c>
       <c r="H29" s="9">
-        <f t="shared" si="4"/>
-        <v>121.695226488</v>
+        <f t="shared" ref="H29:H38" si="5">H7/A7</f>
+        <v>10.9635</v>
       </c>
       <c r="I29" s="9">
-        <f t="shared" si="5"/>
-        <v>52.074639712</v>
+        <f t="shared" ref="I29:I38" si="6">I7/A7</f>
+        <v>5.0392900000000003</v>
       </c>
       <c r="J29" s="9">
-        <f t="shared" si="6"/>
-        <v>122.328619686</v>
+        <f t="shared" ref="J29:J38" si="7">J7/A7</f>
+        <v>22.683689999999999</v>
       </c>
     </row>
     <row r="30" spans="2:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B30" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C30" s="12">
-        <f t="shared" ref="C30:C37" si="7">C9/A9</f>
-        <v>1.1236900000000001</v>
+        <f>C8/A8</f>
+        <v>51.102978159999999</v>
       </c>
       <c r="D30" s="12">
-        <f t="shared" si="0"/>
-        <v>6.4793900000000004</v>
+        <f t="shared" si="1"/>
+        <v>120.145670401</v>
       </c>
       <c r="E30" s="12">
-        <f t="shared" si="1"/>
-        <v>1.81677</v>
+        <f t="shared" si="2"/>
+        <v>51.644393409000003</v>
       </c>
       <c r="F30" s="12">
-        <f t="shared" si="2"/>
-        <v>11.775840000000001</v>
+        <f t="shared" si="3"/>
+        <v>119.56081147800001</v>
       </c>
       <c r="G30" s="12">
-        <f t="shared" si="3"/>
-        <v>5.5166500000000003</v>
+        <f t="shared" si="4"/>
+        <v>51.655900987999999</v>
       </c>
       <c r="H30" s="12">
-        <f t="shared" si="4"/>
-        <v>62.530230000000003</v>
+        <f t="shared" si="5"/>
+        <v>121.695226488</v>
       </c>
       <c r="I30" s="12">
-        <f t="shared" si="5"/>
-        <v>7.90585</v>
+        <f t="shared" si="6"/>
+        <v>52.074639712</v>
       </c>
       <c r="J30" s="12">
-        <f t="shared" si="6"/>
-        <v>1752.7023099999999</v>
+        <f t="shared" si="7"/>
+        <v>122.328619686</v>
       </c>
     </row>
     <row r="31" spans="2:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B31" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C31" s="9">
+        <f t="shared" ref="C31:C38" si="8">C9/A9</f>
+        <v>1.1236900000000001</v>
+      </c>
+      <c r="D31" s="9">
+        <f t="shared" si="1"/>
+        <v>6.4793900000000004</v>
+      </c>
+      <c r="E31" s="9">
+        <f t="shared" si="2"/>
+        <v>1.81677</v>
+      </c>
+      <c r="F31" s="9">
+        <f t="shared" si="3"/>
+        <v>11.775840000000001</v>
+      </c>
+      <c r="G31" s="9">
+        <f t="shared" si="4"/>
+        <v>5.5166500000000003</v>
+      </c>
+      <c r="H31" s="9">
+        <f t="shared" si="5"/>
+        <v>62.530230000000003</v>
+      </c>
+      <c r="I31" s="9">
+        <f t="shared" si="6"/>
+        <v>7.90585</v>
+      </c>
+      <c r="J31" s="9">
         <f t="shared" si="7"/>
-        <v>9.0154158160000009</v>
-      </c>
-      <c r="D31" s="9">
-        <f t="shared" si="0"/>
-        <v>21.340000904</v>
-      </c>
-      <c r="E31" s="9">
-        <f t="shared" si="1"/>
-        <v>9.0774262760000006</v>
-      </c>
-      <c r="F31" s="9">
-        <f t="shared" si="2"/>
-        <v>20.880980393000002</v>
-      </c>
-      <c r="G31" s="9">
-        <f t="shared" si="3"/>
-        <v>9.1983713060000003</v>
-      </c>
-      <c r="H31" s="9">
-        <f t="shared" si="4"/>
-        <v>21.021737761000001</v>
-      </c>
-      <c r="I31" s="9">
-        <f t="shared" si="5"/>
-        <v>9.0003356379999992</v>
-      </c>
-      <c r="J31" s="9">
-        <f t="shared" si="6"/>
-        <v>21.148751373</v>
+        <v>1752.7023099999999</v>
       </c>
     </row>
     <row r="32" spans="2:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B32" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C32" s="12">
+        <f t="shared" si="8"/>
+        <v>9.0154158160000009</v>
+      </c>
+      <c r="D32" s="12">
+        <f t="shared" si="1"/>
+        <v>21.340000904</v>
+      </c>
+      <c r="E32" s="12">
+        <f t="shared" si="2"/>
+        <v>9.0774262760000006</v>
+      </c>
+      <c r="F32" s="12">
+        <f t="shared" si="3"/>
+        <v>20.880980393000002</v>
+      </c>
+      <c r="G32" s="12">
+        <f t="shared" si="4"/>
+        <v>9.1983713060000003</v>
+      </c>
+      <c r="H32" s="12">
+        <f t="shared" si="5"/>
+        <v>21.021737761000001</v>
+      </c>
+      <c r="I32" s="12">
+        <f t="shared" si="6"/>
+        <v>9.0003356379999992</v>
+      </c>
+      <c r="J32" s="12">
         <f t="shared" si="7"/>
-        <v>2.0280999999999998</v>
-      </c>
-      <c r="D32" s="12">
-        <f t="shared" si="0"/>
-        <v>14.775</v>
-      </c>
-      <c r="E32" s="12">
-        <f t="shared" si="1"/>
-        <v>2.8098000000000001</v>
-      </c>
-      <c r="F32" s="12">
-        <f t="shared" si="2"/>
-        <v>13.6333</v>
-      </c>
-      <c r="G32" s="12">
-        <f t="shared" si="3"/>
-        <v>4.8731999999999998</v>
-      </c>
-      <c r="H32" s="12">
-        <f t="shared" si="4"/>
-        <v>24.221599999999999</v>
-      </c>
-      <c r="I32" s="12">
-        <f t="shared" si="5"/>
-        <v>9.02</v>
-      </c>
-      <c r="J32" s="12">
-        <f t="shared" si="6"/>
-        <v>402.34530000000001</v>
+        <v>21.148751373</v>
       </c>
     </row>
     <row r="33" spans="2:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B33" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C33" s="9">
+        <f t="shared" si="8"/>
+        <v>2.0280999999999998</v>
+      </c>
+      <c r="D33" s="9">
+        <f t="shared" si="1"/>
+        <v>14.775</v>
+      </c>
+      <c r="E33" s="9">
+        <f t="shared" si="2"/>
+        <v>2.8098000000000001</v>
+      </c>
+      <c r="F33" s="9">
+        <f t="shared" si="3"/>
+        <v>13.6333</v>
+      </c>
+      <c r="G33" s="9">
+        <f t="shared" si="4"/>
+        <v>4.8731999999999998</v>
+      </c>
+      <c r="H33" s="9">
+        <f t="shared" si="5"/>
+        <v>24.221599999999999</v>
+      </c>
+      <c r="I33" s="9">
+        <f t="shared" si="6"/>
+        <v>9.02</v>
+      </c>
+      <c r="J33" s="9">
         <f t="shared" si="7"/>
-        <v>51.963999999999999</v>
-      </c>
-      <c r="D33" s="9">
-        <f t="shared" si="0"/>
-        <v>83.477000000000004</v>
-      </c>
-      <c r="E33" s="9">
-        <f t="shared" si="1"/>
-        <v>120.095</v>
-      </c>
-      <c r="F33" s="9">
-        <f t="shared" si="2"/>
-        <v>187.55500000000001</v>
-      </c>
-      <c r="G33" s="9">
-        <f t="shared" si="3"/>
-        <v>80.581000000000003</v>
-      </c>
-      <c r="H33" s="9">
-        <f t="shared" si="4"/>
-        <v>108.633</v>
-      </c>
-      <c r="I33" s="9">
-        <f t="shared" si="5"/>
-        <v>51.024000000000001</v>
-      </c>
-      <c r="J33" s="9">
-        <f t="shared" si="6"/>
-        <v>70.037999999999997</v>
+        <v>402.34530000000001</v>
       </c>
     </row>
     <row r="34" spans="2:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B34" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C34" s="12">
+        <f t="shared" si="8"/>
+        <v>51.963999999999999</v>
+      </c>
+      <c r="D34" s="12">
+        <f t="shared" si="1"/>
+        <v>83.477000000000004</v>
+      </c>
+      <c r="E34" s="12">
+        <f t="shared" si="2"/>
+        <v>120.095</v>
+      </c>
+      <c r="F34" s="12">
+        <f t="shared" si="3"/>
+        <v>187.55500000000001</v>
+      </c>
+      <c r="G34" s="12">
+        <f t="shared" si="4"/>
+        <v>80.581000000000003</v>
+      </c>
+      <c r="H34" s="12">
+        <f t="shared" si="5"/>
+        <v>108.633</v>
+      </c>
+      <c r="I34" s="12">
+        <f t="shared" si="6"/>
+        <v>51.024000000000001</v>
+      </c>
+      <c r="J34" s="12">
         <f t="shared" si="7"/>
-        <v>3.8176000000000001</v>
-      </c>
-      <c r="D34" s="12">
-        <f t="shared" si="0"/>
-        <v>7.7121000000000004</v>
-      </c>
-      <c r="E34" s="12">
-        <f t="shared" si="1"/>
-        <v>4.5589000000000004</v>
-      </c>
-      <c r="F34" s="12">
-        <f t="shared" si="2"/>
-        <v>9.4639000000000006</v>
-      </c>
-      <c r="G34" s="12">
-        <f t="shared" si="3"/>
-        <v>6.1604000000000001</v>
-      </c>
-      <c r="H34" s="12">
-        <f t="shared" si="4"/>
-        <v>11.649900000000001</v>
-      </c>
-      <c r="I34" s="12">
-        <f t="shared" si="5"/>
-        <v>9.2798999999999996</v>
-      </c>
-      <c r="J34" s="12">
-        <f t="shared" si="6"/>
-        <v>18.102</v>
+        <v>70.037999999999997</v>
       </c>
     </row>
     <row r="35" spans="2:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B35" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C35" s="9">
+        <f t="shared" si="8"/>
+        <v>3.8176000000000001</v>
+      </c>
+      <c r="D35" s="9">
+        <f t="shared" si="1"/>
+        <v>7.7121000000000004</v>
+      </c>
+      <c r="E35" s="9">
+        <f t="shared" si="2"/>
+        <v>4.5589000000000004</v>
+      </c>
+      <c r="F35" s="9">
+        <f t="shared" si="3"/>
+        <v>9.4639000000000006</v>
+      </c>
+      <c r="G35" s="9">
+        <f t="shared" si="4"/>
+        <v>6.1604000000000001</v>
+      </c>
+      <c r="H35" s="9">
+        <f t="shared" si="5"/>
+        <v>11.649900000000001</v>
+      </c>
+      <c r="I35" s="9">
+        <f t="shared" si="6"/>
+        <v>9.2798999999999996</v>
+      </c>
+      <c r="J35" s="9">
         <f t="shared" si="7"/>
-        <v>87.276443049999997</v>
-      </c>
-      <c r="D35" s="9">
-        <f t="shared" si="0"/>
-        <v>198.90767276</v>
-      </c>
-      <c r="E35" s="9">
-        <f t="shared" si="1"/>
-        <v>90.833824390000004</v>
-      </c>
-      <c r="F35" s="9">
-        <f t="shared" si="2"/>
-        <v>201.60303761</v>
-      </c>
-      <c r="G35" s="9">
-        <f t="shared" si="3"/>
-        <v>98.147187000000002</v>
-      </c>
-      <c r="H35" s="9">
-        <f t="shared" si="4"/>
-        <v>210.43827797</v>
-      </c>
-      <c r="I35" s="9">
-        <f t="shared" si="5"/>
-        <v>110.54716356</v>
-      </c>
-      <c r="J35" s="9">
-        <f t="shared" si="6"/>
-        <v>231.29576940000001</v>
+        <v>18.102</v>
       </c>
     </row>
     <row r="36" spans="2:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B36" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C36" s="12">
+        <f t="shared" si="8"/>
+        <v>87.276443049999997</v>
+      </c>
+      <c r="D36" s="12">
+        <f t="shared" si="1"/>
+        <v>198.90767276</v>
+      </c>
+      <c r="E36" s="12">
+        <f t="shared" si="2"/>
+        <v>90.833824390000004</v>
+      </c>
+      <c r="F36" s="12">
+        <f t="shared" si="3"/>
+        <v>201.60303761</v>
+      </c>
+      <c r="G36" s="12">
+        <f t="shared" si="4"/>
+        <v>98.147187000000002</v>
+      </c>
+      <c r="H36" s="12">
+        <f t="shared" si="5"/>
+        <v>210.43827797</v>
+      </c>
+      <c r="I36" s="12">
+        <f t="shared" si="6"/>
+        <v>110.54716356</v>
+      </c>
+      <c r="J36" s="12">
         <f t="shared" si="7"/>
-        <v>58.3125176</v>
-      </c>
-      <c r="D36" s="12">
-        <f t="shared" si="0"/>
-        <v>125.5069293</v>
-      </c>
-      <c r="E36" s="12">
-        <f t="shared" si="1"/>
-        <v>57.767734300000001</v>
-      </c>
-      <c r="F36" s="12">
-        <f t="shared" si="2"/>
-        <v>125.1732442</v>
-      </c>
-      <c r="G36" s="12">
-        <f t="shared" si="3"/>
-        <v>58.489876199999998</v>
-      </c>
-      <c r="H36" s="12">
-        <f t="shared" si="4"/>
-        <v>125.16341180000001</v>
-      </c>
-      <c r="I36" s="12">
-        <f t="shared" si="5"/>
-        <v>58.892713899999997</v>
-      </c>
-      <c r="J36" s="12">
-        <f t="shared" si="6"/>
-        <v>125.4963592</v>
+        <v>231.29576940000001</v>
       </c>
     </row>
     <row r="37" spans="2:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B37" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C37" s="9">
+        <f t="shared" si="8"/>
+        <v>58.3125176</v>
+      </c>
+      <c r="D37" s="9">
+        <f t="shared" si="1"/>
+        <v>125.5069293</v>
+      </c>
+      <c r="E37" s="9">
+        <f t="shared" si="2"/>
+        <v>57.767734300000001</v>
+      </c>
+      <c r="F37" s="9">
+        <f t="shared" si="3"/>
+        <v>125.1732442</v>
+      </c>
+      <c r="G37" s="9">
+        <f t="shared" si="4"/>
+        <v>58.489876199999998</v>
+      </c>
+      <c r="H37" s="9">
+        <f t="shared" si="5"/>
+        <v>125.16341180000001</v>
+      </c>
+      <c r="I37" s="9">
+        <f t="shared" si="6"/>
+        <v>58.892713899999997</v>
+      </c>
+      <c r="J37" s="9">
+        <f t="shared" si="7"/>
+        <v>125.4963592</v>
+      </c>
+    </row>
+    <row r="38" spans="2:10" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B38" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="C37" s="9">
+      <c r="C38" s="12">
+        <f t="shared" si="8"/>
+        <v>14.994</v>
+      </c>
+      <c r="D38" s="12">
+        <f t="shared" si="1"/>
+        <v>34.063000000000002</v>
+      </c>
+      <c r="E38" s="12">
+        <f t="shared" si="2"/>
+        <v>8.9764999999999997</v>
+      </c>
+      <c r="F38" s="12">
+        <f t="shared" si="3"/>
+        <v>19.8674</v>
+      </c>
+      <c r="G38" s="12">
+        <f t="shared" si="4"/>
+        <v>6.3609</v>
+      </c>
+      <c r="H38" s="12">
+        <f t="shared" si="5"/>
+        <v>13.179600000000001</v>
+      </c>
+      <c r="I38" s="12">
+        <f t="shared" si="6"/>
+        <v>5.3792</v>
+      </c>
+      <c r="J38" s="12">
         <f t="shared" si="7"/>
-        <v>14.994</v>
-      </c>
-      <c r="D37" s="9">
-        <f t="shared" si="0"/>
-        <v>34.063000000000002</v>
-      </c>
-      <c r="E37" s="9">
-        <f t="shared" si="1"/>
-        <v>8.9764999999999997</v>
-      </c>
-      <c r="F37" s="9">
-        <f t="shared" si="2"/>
-        <v>19.8674</v>
-      </c>
-      <c r="G37" s="9">
-        <f t="shared" si="3"/>
-        <v>6.3609</v>
-      </c>
-      <c r="H37" s="9">
-        <f t="shared" si="4"/>
-        <v>13.179600000000001</v>
-      </c>
-      <c r="I37" s="9">
-        <f t="shared" si="5"/>
-        <v>5.3792</v>
-      </c>
-      <c r="J37" s="9">
-        <f t="shared" si="6"/>
         <v>11.632</v>
       </c>
     </row>

</xml_diff>